<commit_message>
Atualização automática da planilha via Apps Script 003
</commit_message>
<xml_diff>
--- a/Controle_Lote_Validade.xlsx
+++ b/Controle_Lote_Validade.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="EstoqueSolicitacao" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Lotes" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">EstoqueSolicitacao!$B$1:$W$319</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Lotes!$B$1:$W$319</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -1185,8 +1185,8 @@
         <v>0</v>
       </c>
       <c r="P11" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),259.0)</f>
-        <v>259</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),257.0)</f>
+        <v>257</v>
       </c>
       <c r="Q11" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-2.0)</f>
@@ -1854,8 +1854,8 @@
         <v>0</v>
       </c>
       <c r="P20" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),222.0)</f>
-        <v>222</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),220.0)</f>
+        <v>220</v>
       </c>
       <c r="Q20" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -2219,8 +2219,8 @@
         <v>0</v>
       </c>
       <c r="P25" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),396.0)</f>
-        <v>396</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),392.0)</f>
+        <v>392</v>
       </c>
       <c r="Q25" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -2371,8 +2371,8 @@
         <v>0</v>
       </c>
       <c r="P27" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),301.0)</f>
-        <v>301</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),297.0)</f>
+        <v>297</v>
       </c>
       <c r="Q27" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -2599,8 +2599,8 @@
         <v>0</v>
       </c>
       <c r="P30" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),519.0)</f>
-        <v>519</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),513.0)</f>
+        <v>513</v>
       </c>
       <c r="Q30" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -3390,8 +3390,8 @@
         <v>0</v>
       </c>
       <c r="P41" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),276.0)</f>
-        <v>276</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),266.0)</f>
+        <v>266</v>
       </c>
       <c r="Q41" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -4433,8 +4433,8 @@
         <v>0</v>
       </c>
       <c r="P55" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),188.0)</f>
-        <v>188</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),186.0)</f>
+        <v>186</v>
       </c>
       <c r="Q55" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -5403,8 +5403,8 @@
         <v>0</v>
       </c>
       <c r="P68" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),197.0)</f>
-        <v>197</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),195.0)</f>
+        <v>195</v>
       </c>
       <c r="Q68" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -5631,8 +5631,8 @@
         <v>0</v>
       </c>
       <c r="P71" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),235.0)</f>
-        <v>235</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),225.0)</f>
+        <v>225</v>
       </c>
       <c r="Q71" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -5853,8 +5853,8 @@
         <v>0</v>
       </c>
       <c r="P74" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),212.0)</f>
-        <v>212</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),208.0)</f>
+        <v>208</v>
       </c>
       <c r="Q74" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -7623,8 +7623,8 @@
         <v>0</v>
       </c>
       <c r="P98" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),566.0)</f>
-        <v>566</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),562.0)</f>
+        <v>562</v>
       </c>
       <c r="Q98" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -7699,8 +7699,8 @@
         <v>0</v>
       </c>
       <c r="P99" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),444.0)</f>
-        <v>444</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),432.0)</f>
+        <v>432</v>
       </c>
       <c r="Q99" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
@@ -7775,8 +7775,8 @@
         <v>0</v>
       </c>
       <c r="P100" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),199.0)</f>
-        <v>199</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),195.0)</f>
+        <v>195</v>
       </c>
       <c r="Q100" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -8003,8 +8003,8 @@
         <v>0</v>
       </c>
       <c r="P103" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),247.0)</f>
-        <v>247</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),245.0)</f>
+        <v>245</v>
       </c>
       <c r="Q103" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -8152,12 +8152,12 @@
         <v>0</v>
       </c>
       <c r="P105" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),732.0)</f>
-        <v>732</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),728.0)</f>
+        <v>728</v>
       </c>
       <c r="Q105" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
       <c r="R105" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3500.0)</f>
@@ -8304,8 +8304,8 @@
         <v>0</v>
       </c>
       <c r="P107" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),604.0)</f>
-        <v>604</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),598.0)</f>
+        <v>598</v>
       </c>
       <c r="Q107" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
@@ -8608,8 +8608,8 @@
         <v>0</v>
       </c>
       <c r="P111" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
-        <v>79</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),77.0)</f>
+        <v>77</v>
       </c>
       <c r="Q111" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.0)</f>
@@ -8678,8 +8678,8 @@
         <v>0</v>
       </c>
       <c r="P112" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
-        <v>79</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),77.0)</f>
+        <v>77</v>
       </c>
       <c r="Q112" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.0)</f>
@@ -9800,12 +9800,12 @@
         <v>0</v>
       </c>
       <c r="P127" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),583.0)</f>
-        <v>583</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),579.0)</f>
+        <v>579</v>
       </c>
       <c r="Q127" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
-        <v>34</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
+        <v>38</v>
       </c>
       <c r="R127" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2000.0)</f>
@@ -17106,8 +17106,8 @@
         <v>0</v>
       </c>
       <c r="P227" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),144.0)</f>
-        <v>144</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),138.0)</f>
+        <v>138</v>
       </c>
       <c r="Q227" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-10.0)</f>
@@ -19226,8 +19226,8 @@
         <v>600</v>
       </c>
       <c r="P256" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),298.0)</f>
-        <v>298</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),292.0)</f>
+        <v>292</v>
       </c>
       <c r="Q256" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
@@ -20619,12 +20619,12 @@
         <v>700</v>
       </c>
       <c r="P275" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),987.0)</f>
-        <v>987</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),985.0)</f>
+        <v>985</v>
       </c>
       <c r="Q275" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),92.0)</f>
-        <v>92</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),94.0)</f>
+        <v>94</v>
       </c>
       <c r="R275" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3000.0)</f>
@@ -22544,12 +22544,12 @@
         <v>1100</v>
       </c>
       <c r="P301" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),548.0)</f>
-        <v>548</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),542.0)</f>
+        <v>542</v>
       </c>
       <c r="Q301" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
       </c>
       <c r="R301" s="7"/>
       <c r="S301" s="5"/>
@@ -23277,8 +23277,8 @@
         <v>1100</v>
       </c>
       <c r="P311" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),468.0)</f>
-        <v>468</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),460.0)</f>
+        <v>460</v>
       </c>
       <c r="Q311" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),-18.0)</f>
@@ -23423,8 +23423,8 @@
         <v>1500</v>
       </c>
       <c r="P313" s="7">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),238.0)</f>
-        <v>238</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),236.0)</f>
+        <v>236</v>
       </c>
       <c r="Q313" s="7">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>

</xml_diff>